<commit_message>
Driver is now from katalon and test cases run in katalon with selenium
</commit_message>
<xml_diff>
--- a/CTDC_Automation/TestData/Password_canineKatalon.xlsx
+++ b/CTDC_Automation/TestData/Password_canineKatalon.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\Script\DataCommons_Automation\CTDC_Automation\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laxmi\Katalone_recent_code\DataCommons_Automation\CTDC_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D1C13FF-4C69-416F-A7C0-ACD1FA0FDEE6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA96F108-7F1A-4DA5-80E2-A5CE0FA9D7E1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
   <sheets>
     <sheet name="startup" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="115">
   <si>
     <t>Environment</t>
   </si>
@@ -368,9 +368,6 @@
   </si>
   <si>
     <t>Neo4jData_canineKatalon_TC1.xlsx</t>
-  </si>
-  <si>
-    <t>https://caninecommons-qa.cancer.gov/#/</t>
   </si>
   <si>
     <t>tblbody</t>
@@ -763,23 +760,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.453125" customWidth="1"/>
-    <col min="4" max="4" width="59.26953125" customWidth="1"/>
-    <col min="6" max="6" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="75.81640625" customWidth="1"/>
-    <col min="9" max="9" width="70.26953125" customWidth="1"/>
-    <col min="10" max="10" width="28.54296875" customWidth="1"/>
+    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.42578125" customWidth="1"/>
+    <col min="4" max="4" width="59.28515625" customWidth="1"/>
+    <col min="6" max="6" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="75.85546875" customWidth="1"/>
+    <col min="9" max="9" width="70.28515625" customWidth="1"/>
+    <col min="10" max="10" width="28.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -802,21 +799,21 @@
         <v>108</v>
       </c>
       <c r="H1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="J1" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="159.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" ht="165" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>112</v>
+        <v>25</v>
       </c>
       <c r="C2" t="s">
         <v>107</v>
@@ -834,7 +831,7 @@
         <v>109</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I2" t="s">
         <v>111</v>
@@ -862,15 +859,15 @@
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="79.7265625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="79.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D1" s="1" t="s">
         <v>101</v>
       </c>
@@ -878,12 +875,12 @@
         <v>100</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D2" s="1" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
         <v>106</v>
       </c>
@@ -897,7 +894,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D4" t="s">
         <v>105</v>
       </c>
@@ -905,7 +902,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1</v>
       </c>
@@ -922,7 +919,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>29</v>
       </c>
@@ -933,7 +930,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>33</v>
       </c>
@@ -941,7 +938,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>35</v>
       </c>
@@ -949,12 +946,12 @@
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="4:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D21" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="23" spans="4:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D23" t="s">
         <v>31</v>
       </c>
@@ -962,42 +959,42 @@
         <v>38</v>
       </c>
     </row>
-    <row r="26" spans="4:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D26" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="28" spans="4:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D28" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="31" spans="4:5" x14ac:dyDescent="0.35">
+    <row r="31" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D31" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="32" spans="4:5" x14ac:dyDescent="0.35">
+    <row r="32" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D32" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="34" spans="4:6" x14ac:dyDescent="0.35">
+    <row r="34" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D34" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="38" spans="4:6" x14ac:dyDescent="0.35">
+    <row r="38" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D38" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="39" spans="4:6" x14ac:dyDescent="0.35">
+    <row r="39" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D39" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="40" spans="4:6" x14ac:dyDescent="0.35">
+    <row r="40" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D40" t="s">
         <v>44</v>
       </c>
@@ -1005,12 +1002,12 @@
         <v>47</v>
       </c>
     </row>
-    <row r="41" spans="4:6" x14ac:dyDescent="0.35">
+    <row r="41" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D41" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="43" spans="4:6" x14ac:dyDescent="0.35">
+    <row r="43" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D43" t="s">
         <v>44</v>
       </c>
@@ -1018,17 +1015,17 @@
         <v>49</v>
       </c>
     </row>
-    <row r="45" spans="4:6" x14ac:dyDescent="0.35">
+    <row r="45" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D45" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="4:6" x14ac:dyDescent="0.35">
+    <row r="47" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D47" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C50" t="s">
         <v>53</v>
       </c>
@@ -1039,7 +1036,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D51" s="2" t="s">
         <v>52</v>
       </c>
@@ -1050,7 +1047,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="J52" t="s">
         <v>51</v>
       </c>
@@ -1058,7 +1055,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="J53" t="s">
         <v>18</v>
       </c>
@@ -1066,7 +1063,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="J54" t="s">
         <v>18</v>
       </c>
@@ -1074,7 +1071,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>3</v>
       </c>
@@ -1106,7 +1103,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>3</v>
       </c>
@@ -1135,7 +1132,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>3</v>
       </c>
@@ -1164,7 +1161,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>3</v>
       </c>
@@ -1199,7 +1196,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>3</v>
       </c>
@@ -1234,7 +1231,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>3</v>
       </c>
@@ -1269,7 +1266,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="J61" t="s">
         <v>18</v>
       </c>
@@ -1277,7 +1274,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="J62" t="s">
         <v>14</v>
       </c>
@@ -1285,7 +1282,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>3</v>
       </c>
@@ -1320,7 +1317,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>3</v>
       </c>
@@ -1355,7 +1352,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>3</v>
       </c>
@@ -1390,7 +1387,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>3</v>
       </c>
@@ -1425,7 +1422,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>17</v>
       </c>
@@ -1460,7 +1457,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>17</v>
       </c>
@@ -1495,7 +1492,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>3</v>
       </c>
@@ -1530,7 +1527,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>3</v>
       </c>
@@ -1565,7 +1562,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>17</v>
       </c>
@@ -1600,7 +1597,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>3</v>
       </c>
@@ -1629,7 +1626,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>3</v>
       </c>
@@ -1658,7 +1655,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>3</v>
       </c>
@@ -1687,7 +1684,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>3</v>
       </c>
@@ -1716,7 +1713,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>3</v>
       </c>
@@ -1745,12 +1742,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C78" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C81" t="s">
         <v>84</v>
       </c>
@@ -1758,7 +1755,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C82" t="s">
         <v>78</v>
       </c>
@@ -1766,7 +1763,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C83" t="s">
         <v>87</v>
       </c>
@@ -1774,7 +1771,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C84" t="s">
         <v>89</v>
       </c>
@@ -1788,7 +1785,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C85" t="s">
         <v>81</v>
       </c>
@@ -1796,7 +1793,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C86" t="s">
         <v>91</v>
       </c>
@@ -1804,7 +1801,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C87" t="s">
         <v>93</v>
       </c>
@@ -1812,7 +1809,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>3</v>
       </c>
@@ -1847,7 +1844,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="J90" t="s">
         <v>18</v>
       </c>
@@ -1855,7 +1852,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="J91" t="s">
         <v>18</v>
       </c>
@@ -1863,7 +1860,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="J92" t="s">
         <v>18</v>
       </c>
@@ -1871,7 +1868,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="J93" t="s">
         <v>72</v>
       </c>
@@ -1879,7 +1876,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>3</v>
       </c>
@@ -1914,7 +1911,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>3</v>
       </c>
@@ -1949,7 +1946,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>3</v>
       </c>
@@ -1984,7 +1981,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>3</v>
       </c>
@@ -2013,7 +2010,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>17</v>
       </c>
@@ -2042,7 +2039,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>17</v>
       </c>
@@ -2071,7 +2068,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>17</v>
       </c>
@@ -2100,7 +2097,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>17</v>
       </c>

</xml_diff>